<commit_message>
[Review] 하네스 current, 사용시간
</commit_message>
<xml_diff>
--- a/1_Plasma_Pipette/4_Review data/Plasma_Pipette Review Data.xlsx
+++ b/1_Plasma_Pipette/4_Review data/Plasma_Pipette Review Data.xlsx
@@ -4,23 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="하네스" sheetId="3" r:id="rId1"/>
     <sheet name="ME Size" sheetId="1" r:id="rId2"/>
     <sheet name="Battery CON" sheetId="2" r:id="rId3"/>
     <sheet name="Power review" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
-    <sheet name="LED" sheetId="6" r:id="rId6"/>
-    <sheet name="SV" sheetId="7" r:id="rId7"/>
+    <sheet name="LED" sheetId="6" r:id="rId5"/>
+    <sheet name="SV" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="172">
   <si>
     <t>Battery 용량</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -170,10 +170,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Transformer PCB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>S/V</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -490,43 +486,231 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>Open</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Operation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Closed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delay  발생</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Icc[A]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vcc[V]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>S/V review data</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Data - No bias resistor</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>X605SF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>912-000007-009</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>X605SF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Open</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Operation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Closed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Delay  발생</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Icc[A]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Vcc[V]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>S/V review data</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test Data - No bias resistor</t>
+    <t>Main PCB
+V1.0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transformer PCB
+V2.0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Main PCB
+V2.0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MCU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status LED</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma ON LED</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power Level LED</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transformer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>S/V</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Idle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ON</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OFF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma On</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Current[mA]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery 용량</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mAh</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hour</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Minute</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma
+On</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Current
+[mA]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>각  Block별  소모전류</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>각 mode별 current</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery 용량에 따른 사용 시간</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status LED</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma LED</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma Level LED</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ω</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AWG Spec</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AWG</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>허용 전류</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>실리콘</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>저항</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>Ω</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/km</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ω/0.1m</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전압 drop</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.5A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPB605060</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -534,11 +718,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="177" formatCode="0.0\ &quot;%&quot;"/>
+    <numFmt numFmtId="181" formatCode="0.00000"/>
+    <numFmt numFmtId="183" formatCode="0.000"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -728,8 +915,23 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -927,8 +1129,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -1325,6 +1533,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1484,7 +1757,7 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1604,42 +1877,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1657,6 +1894,261 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="15" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="20" fillId="33" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="20" fillId="33" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="20% - 강조색1" xfId="17" builtinId="30" customBuiltin="1"/>
@@ -1716,6 +2208,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF66FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1732,15 +2229,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>3134519</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>134257</xdr:rowOff>
+      <xdr:colOff>3344069</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>143782</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1757,7 +2254,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7820025" y="6972300"/>
+          <a:off x="8029575" y="10629900"/>
           <a:ext cx="5687219" cy="6496957"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1774,16 +2271,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>200025</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1807,7 +2304,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1143000" y="619125"/>
+          <a:off x="10210800" y="647700"/>
           <a:ext cx="4238625" cy="4381500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2117,10 +2614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L38"/>
+  <dimension ref="B1:L54"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2145,10 +2642,10 @@
     </row>
     <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2167,29 +2664,29 @@
         <v>29</v>
       </c>
       <c r="I3" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J3" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="17" t="s">
-        <v>40</v>
-      </c>
       <c r="L3" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="69" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="36">
+      <c r="B4" s="90" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="91">
         <v>1</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="69" t="s">
+      <c r="E4" s="81" t="s">
         <v>26</v>
       </c>
       <c r="F4" s="36">
@@ -2202,81 +2699,95 @@
         <v>23</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="70"/>
-      <c r="C5" s="32">
+      <c r="B5" s="93"/>
+      <c r="C5" s="94">
         <v>2</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="70"/>
+      <c r="E5" s="82"/>
       <c r="F5" s="32">
         <v>2</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="67" t="s">
-        <v>49</v>
+      <c r="I5" s="79" t="s">
+        <v>48</v>
       </c>
       <c r="J5" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="L5" s="37" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="71"/>
-      <c r="C6" s="19">
+      <c r="B6" s="96"/>
+      <c r="C6" s="97">
         <v>3</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="71"/>
+      <c r="E6" s="83"/>
       <c r="F6" s="19">
         <v>3</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="67"/>
+      <c r="I6" s="79"/>
       <c r="J6" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="K6" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="K6" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" s="37" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I7" s="67"/>
+    </row>
+    <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I7" s="79"/>
       <c r="J7" s="41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I8" s="68"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="33"/>
+      <c r="F8" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="80"/>
       <c r="J8" s="7" t="s">
         <v>26</v>
       </c>
@@ -2284,8 +2795,23 @@
       <c r="L8" s="8"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="11" t="s">
-        <v>27</v>
+      <c r="B9" s="89" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="36">
+        <v>3</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="81" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="36">
+        <v>1</v>
+      </c>
+      <c r="G9" s="50" t="s">
+        <v>24</v>
       </c>
       <c r="I9" s="15"/>
       <c r="J9" s="9"/>
@@ -2293,532 +2819,714 @@
       <c r="L9" s="9"/>
     </row>
     <row r="10" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="82"/>
+      <c r="C10" s="32">
+        <v>2</v>
+      </c>
+      <c r="D10" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="82"/>
+      <c r="F10" s="32">
+        <v>2</v>
+      </c>
+      <c r="G10" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="11" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="33"/>
-      <c r="C11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="33"/>
-      <c r="F11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>29</v>
+      <c r="B11" s="83"/>
+      <c r="C11" s="19">
+        <v>1</v>
+      </c>
+      <c r="D11" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="83"/>
+      <c r="F11" s="19">
+        <v>3</v>
+      </c>
+      <c r="G11" s="52" t="s">
+        <v>31</v>
       </c>
       <c r="I11" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J11" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="K11" s="17" t="s">
-        <v>40</v>
-      </c>
       <c r="L11" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="36">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="64" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="36">
-        <v>1</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="I12" s="34" t="s">
         <v>23</v>
       </c>
       <c r="J12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="65"/>
-      <c r="C13" s="32">
-        <v>2</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="65"/>
-      <c r="F13" s="32">
-        <v>2</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="67" t="s">
+      <c r="I13" s="79" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="J13" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="L13" s="37" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="65"/>
-      <c r="C14" s="32">
-        <v>3</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="65" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="32">
-        <v>1</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="67"/>
+      <c r="B14" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="79"/>
       <c r="J14" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L14" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="K14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="L14" s="37" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="65"/>
-      <c r="C15" s="32">
-        <v>4</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="65"/>
-      <c r="F15" s="32">
-        <v>2</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I15" s="67"/>
+    </row>
+    <row r="15" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" s="79"/>
       <c r="J15" s="41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="33"/>
+      <c r="C16" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="33"/>
+      <c r="F16" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="79"/>
+      <c r="J16" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L16" s="37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="99" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="91">
+        <v>1</v>
+      </c>
+      <c r="D17" s="92" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="36">
+        <v>1</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="79"/>
+      <c r="J17" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L17" s="37" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="65"/>
-      <c r="C16" s="32">
-        <v>5</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="65"/>
-      <c r="F16" s="32">
-        <v>3</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I16" s="67"/>
-      <c r="J16" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="L16" s="37" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="65"/>
-      <c r="C17" s="32">
-        <v>6</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="65"/>
-      <c r="F17" s="32">
-        <v>4</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I17" s="67"/>
-      <c r="J17" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="L17" s="37" t="s">
-        <v>55</v>
-      </c>
-    </row>
     <row r="18" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="66"/>
-      <c r="C18" s="19">
-        <v>7</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="66"/>
-      <c r="F18" s="19">
-        <v>5</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>35</v>
+      <c r="B18" s="100"/>
+      <c r="C18" s="94">
+        <v>2</v>
+      </c>
+      <c r="D18" s="95" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="77"/>
+      <c r="F18" s="32">
+        <v>2</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="I18" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L18" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="L18" s="8" t="s">
-        <v>44</v>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B19" s="100"/>
+      <c r="C19" s="94">
+        <v>3</v>
+      </c>
+      <c r="D19" s="95" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="88" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="32">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B20" s="11" t="s">
-        <v>64</v>
+      <c r="B20" s="100"/>
+      <c r="C20" s="94">
+        <v>4</v>
+      </c>
+      <c r="D20" s="95" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="77"/>
+      <c r="F20" s="32">
+        <v>2</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="100"/>
+      <c r="C21" s="94">
+        <v>5</v>
+      </c>
+      <c r="D21" s="95" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="77"/>
+      <c r="F21" s="32">
+        <v>3</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="22" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="33"/>
-      <c r="C22" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="33"/>
-      <c r="F22" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="24" t="s">
-        <v>29</v>
+      <c r="B22" s="100"/>
+      <c r="C22" s="94">
+        <v>6</v>
+      </c>
+      <c r="D22" s="95" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="77"/>
+      <c r="F22" s="32">
+        <v>4</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="I22" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J22" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="K22" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="K22" s="17" t="s">
-        <v>40</v>
-      </c>
       <c r="L22" s="24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B23" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="36">
-        <v>1</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" s="25"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="13"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="101"/>
+      <c r="C23" s="97">
+        <v>7</v>
+      </c>
+      <c r="D23" s="102" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="78"/>
+      <c r="F23" s="19">
+        <v>5</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="I23" s="34" t="s">
         <v>23</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K23" s="3"/>
       <c r="L23" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I24" s="79" t="s">
+        <v>48</v>
+      </c>
+      <c r="J24" s="43" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B24" s="65"/>
-      <c r="C24" s="32">
-        <v>2</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="21"/>
-      <c r="I24" s="67" t="s">
-        <v>49</v>
-      </c>
-      <c r="J24" s="43" t="s">
+      <c r="K24" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="K24" s="44" t="s">
+      <c r="L24" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="L24" s="37" t="s">
+    </row>
+    <row r="25" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="33"/>
+      <c r="C25" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="33"/>
+      <c r="F25" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" s="79"/>
+      <c r="J25" s="44" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B25" s="65"/>
-      <c r="C25" s="32">
-        <v>3</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" s="65" t="s">
-        <v>70</v>
-      </c>
-      <c r="F25" s="32">
-        <v>1</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="I25" s="67"/>
-      <c r="J25" s="44" t="s">
-        <v>76</v>
       </c>
       <c r="K25" s="5"/>
       <c r="L25" s="29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="65"/>
-      <c r="C26" s="32">
-        <v>4</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" s="65"/>
-      <c r="F26" s="32">
-        <v>2</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="I26" s="68"/>
+      <c r="B26" s="87" t="s">
+        <v>133</v>
+      </c>
+      <c r="C26" s="36">
+        <v>7</v>
+      </c>
+      <c r="D26" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="36">
+        <v>1</v>
+      </c>
+      <c r="G26" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="80"/>
       <c r="J26" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K26" s="7"/>
       <c r="L26" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B27" s="65"/>
+      <c r="B27" s="77"/>
       <c r="C27" s="32">
+        <v>6</v>
+      </c>
+      <c r="D27" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="77"/>
+      <c r="F27" s="32">
+        <v>2</v>
+      </c>
+      <c r="G27" s="51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B28" s="77"/>
+      <c r="C28" s="32">
         <v>5</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D28" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="88" t="s">
+        <v>132</v>
+      </c>
+      <c r="F28" s="32">
+        <v>1</v>
+      </c>
+      <c r="G28" s="51" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B29" s="77"/>
+      <c r="C29" s="32">
+        <v>4</v>
+      </c>
+      <c r="D29" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="77"/>
+      <c r="F29" s="32">
+        <v>2</v>
+      </c>
+      <c r="G29" s="51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B30" s="77"/>
+      <c r="C30" s="32">
+        <v>3</v>
+      </c>
+      <c r="D30" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="77"/>
+      <c r="F30" s="32">
+        <v>3</v>
+      </c>
+      <c r="G30" s="51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B31" s="77"/>
+      <c r="C31" s="32">
+        <v>2</v>
+      </c>
+      <c r="D31" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="77"/>
+      <c r="F31" s="32">
+        <v>4</v>
+      </c>
+      <c r="G31" s="51" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="78"/>
+      <c r="C32" s="19">
+        <v>1</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="78"/>
+      <c r="F32" s="19">
+        <v>5</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="33"/>
+      <c r="C37" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="33"/>
+      <c r="F37" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G37" s="24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B38" s="76" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="36">
+        <v>1</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E38" s="25"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="13"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B39" s="77"/>
+      <c r="C39" s="32">
+        <v>2</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" s="16"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="21"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B40" s="77"/>
+      <c r="C40" s="32">
+        <v>3</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" s="77" t="s">
+        <v>69</v>
+      </c>
+      <c r="F40" s="32">
+        <v>1</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B41" s="77"/>
+      <c r="C41" s="32">
+        <v>4</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E27" s="22"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="35"/>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B28" s="65"/>
-      <c r="C28" s="32">
+      <c r="E41" s="77"/>
+      <c r="F41" s="32">
+        <v>2</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B42" s="77"/>
+      <c r="C42" s="32">
+        <v>5</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42" s="22"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="35"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="77"/>
+      <c r="C43" s="32">
         <v>6</v>
       </c>
-      <c r="D28" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="22"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="21"/>
-    </row>
-    <row r="29" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="66"/>
-      <c r="C29" s="19">
+      <c r="D43" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" s="22"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="21"/>
+    </row>
+    <row r="44" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="78"/>
+      <c r="C44" s="19">
         <v>7</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="27"/>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B31" s="11" t="s">
+      <c r="D44" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E44" s="12"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="27"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B47" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="33"/>
+      <c r="C49" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E49" s="33"/>
+      <c r="F49" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G49" s="24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B50" s="76" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="36">
+        <v>1</v>
+      </c>
+      <c r="D50" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="32" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="33"/>
-      <c r="C33" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D33" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" s="33"/>
-      <c r="F33" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G33" s="24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="36">
-        <v>1</v>
-      </c>
-      <c r="D34" s="4" t="s">
+      <c r="E50" s="76" t="s">
+        <v>84</v>
+      </c>
+      <c r="F50" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B51" s="77"/>
+      <c r="C51" s="32">
+        <v>2</v>
+      </c>
+      <c r="D51" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="64" t="s">
-        <v>85</v>
-      </c>
-      <c r="F34" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="65"/>
-      <c r="C35" s="32">
-        <v>2</v>
-      </c>
-      <c r="D35" s="6" t="s">
+      <c r="E51" s="77"/>
+      <c r="F51" s="32">
+        <v>7</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B52" s="77"/>
+      <c r="C52" s="32">
+        <v>3</v>
+      </c>
+      <c r="D52" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E35" s="65"/>
-      <c r="F35" s="32">
-        <v>7</v>
-      </c>
-      <c r="G35" s="6" t="s">
+      <c r="E52" s="77"/>
+      <c r="F52" s="32">
+        <v>9</v>
+      </c>
+      <c r="G52" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="65"/>
-      <c r="C36" s="32">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B53" s="77"/>
+      <c r="C53" s="32">
+        <v>4</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E53" s="77"/>
+      <c r="F53" s="32">
         <v>3</v>
       </c>
-      <c r="D36" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E36" s="65"/>
-      <c r="F36" s="32">
-        <v>9</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="65"/>
-      <c r="C37" s="32">
+      <c r="G53" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="78"/>
+      <c r="C54" s="19">
+        <v>5</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E54" s="78"/>
+      <c r="F54" s="19">
         <v>4</v>
       </c>
-      <c r="D37" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="32">
-        <v>3</v>
-      </c>
-      <c r="G37" s="6" t="s">
+      <c r="G54" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="66"/>
-      <c r="C38" s="19">
-        <v>5</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E38" s="66"/>
-      <c r="F38" s="19">
-        <v>4</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="E34:E38"/>
+  <mergeCells count="17">
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="B50:B54"/>
+    <mergeCell ref="E50:E54"/>
     <mergeCell ref="I5:I8"/>
     <mergeCell ref="I13:I17"/>
-    <mergeCell ref="B23:B29"/>
-    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="B38:B44"/>
+    <mergeCell ref="E40:E41"/>
     <mergeCell ref="I24:I26"/>
     <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="E14:E18"/>
-    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B17:B23"/>
+    <mergeCell ref="E19:E23"/>
+    <mergeCell ref="E17:E18"/>
     <mergeCell ref="E4:E6"/>
+    <mergeCell ref="B26:B32"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="E28:E32"/>
+    <mergeCell ref="B9:B11"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2828,20 +3536,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:I19"/>
+  <dimension ref="B3:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>5</v>
       </c>
@@ -2858,106 +3569,120 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C5">
+    <row r="5" spans="2:8" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="45">
+        <v>2000</v>
+      </c>
+      <c r="D5" s="45">
+        <v>50</v>
+      </c>
+      <c r="E5" s="45">
+        <v>60</v>
+      </c>
+      <c r="F5" s="45">
+        <v>6</v>
+      </c>
+      <c r="G5" s="45">
+        <f>D5*E5*F5</f>
+        <v>18000</v>
+      </c>
+      <c r="H5" s="45" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C6">
         <v>750</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>48</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>45</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>3</v>
-      </c>
-      <c r="G5">
-        <f>D5*E5*F5</f>
-        <v>6480</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D6">
-        <v>20</v>
-      </c>
-      <c r="E6">
-        <v>90</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
       </c>
       <c r="G6">
         <f>D6*E6*F6</f>
+        <v>6480</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>90</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <f>D7*E7*F7</f>
         <v>18000</v>
       </c>
-      <c r="H6">
-        <f>G6/G5</f>
-        <v>2.7777777777777777</v>
-      </c>
-      <c r="I6">
-        <f>C5*H6</f>
-        <v>2083.3333333333335</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D11" t="s">
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8">
+        <v>51</v>
+      </c>
+      <c r="F8">
+        <v>13</v>
+      </c>
+      <c r="G8" s="45">
+        <f>D8*E8*F8</f>
+        <v>21216</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>2</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C12" t="s">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
         <v>6</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>24</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>68</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
         <v>7</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <v>20</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>90</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>13</v>
-      </c>
-      <c r="D14">
-        <v>30</v>
-      </c>
-      <c r="E14">
-        <v>100</v>
-      </c>
-      <c r="F14">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
-        <v>14</v>
       </c>
       <c r="D15">
         <v>30</v>
@@ -2969,30 +3694,44 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>30</v>
+      </c>
+      <c r="E16">
+        <v>100</v>
+      </c>
+      <c r="F16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18">
-        <v>4</v>
-      </c>
-      <c r="F18" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
         <v>10</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>9</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3113,561 +3852,945 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:P22"/>
+  <dimension ref="A3:R31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13" style="45" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9" style="45"/>
-    <col min="9" max="9" width="5.125" customWidth="1"/>
-    <col min="10" max="10" width="12.875" style="46" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" style="45"/>
+    <col min="2" max="2" width="6.25" customWidth="1"/>
+    <col min="3" max="3" width="13" style="45" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9" style="45"/>
+    <col min="10" max="10" width="5.125" customWidth="1"/>
+    <col min="12" max="12" width="9.625" customWidth="1"/>
+    <col min="13" max="13" width="9.625" style="45" customWidth="1"/>
+    <col min="14" max="14" width="12.25" style="45" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="12.25" style="45" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" customWidth="1"/>
+    <col min="18" max="18" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="I3" s="46" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="72" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" s="47">
-        <v>4</v>
-      </c>
-      <c r="E4" s="61">
+        <v>103</v>
+      </c>
+      <c r="L3" s="46" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C4" s="84" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="47">
         <v>4</v>
       </c>
       <c r="F4" s="61">
         <v>4</v>
       </c>
-      <c r="G4" s="50" t="s">
+      <c r="G4" s="61">
+        <v>4</v>
+      </c>
+      <c r="H4" s="161" t="s">
+        <v>96</v>
+      </c>
+      <c r="L4" s="129"/>
+      <c r="M4" s="130"/>
+      <c r="N4" s="156" t="s">
+        <v>153</v>
+      </c>
+      <c r="O4" s="131" t="s">
+        <v>140</v>
+      </c>
+      <c r="P4" s="132"/>
+      <c r="Q4" s="133" t="s">
+        <v>143</v>
+      </c>
+      <c r="R4" s="134"/>
+    </row>
+    <row r="5" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="85"/>
+      <c r="D5" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="J4" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="K4" s="59">
-        <v>1000</v>
-      </c>
-      <c r="L4" s="60" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B5" s="73"/>
-      <c r="C5" s="48" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="48">
+      <c r="E5" s="48">
         <v>2</v>
-      </c>
-      <c r="E5" s="62">
-        <v>2.5</v>
       </c>
       <c r="F5" s="62">
         <v>2.5</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="62">
+        <v>2.5</v>
+      </c>
+      <c r="H5" s="162" t="s">
+        <v>98</v>
+      </c>
+      <c r="L5" s="135"/>
+      <c r="M5" s="136"/>
+      <c r="N5" s="137"/>
+      <c r="O5" s="138" t="s">
+        <v>145</v>
+      </c>
+      <c r="P5" s="139" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q5" s="140" t="s">
+        <v>145</v>
+      </c>
+      <c r="R5" s="141" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="86"/>
+      <c r="D6" s="49" t="s">
         <v>99</v>
-      </c>
-      <c r="J5" s="54" t="s">
-        <v>98</v>
-      </c>
-      <c r="K5" s="47">
-        <v>2</v>
-      </c>
-      <c r="L5" s="47">
-        <v>2</v>
-      </c>
-      <c r="M5" s="47">
-        <v>2</v>
-      </c>
-      <c r="N5" s="47">
-        <v>2</v>
-      </c>
-      <c r="O5" s="47">
-        <v>2</v>
-      </c>
-      <c r="P5" s="50" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="74"/>
-      <c r="C6" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" s="49">
-        <f>D4*D5</f>
-        <v>8</v>
       </c>
       <c r="E6" s="49">
         <f>E4*E5</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F6" s="49">
         <f>F4*F5</f>
         <v>10</v>
       </c>
-      <c r="G6" s="52" t="s">
-        <v>92</v>
-      </c>
-      <c r="J6" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="K6" s="48">
-        <v>20</v>
-      </c>
-      <c r="L6" s="48">
-        <v>40</v>
-      </c>
-      <c r="M6" s="48">
-        <v>60</v>
-      </c>
-      <c r="N6" s="48">
-        <v>80</v>
-      </c>
-      <c r="O6" s="48">
-        <v>100</v>
-      </c>
-      <c r="P6" s="51" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B7" s="72" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="47">
-        <v>8</v>
-      </c>
-      <c r="E7" s="61">
+      <c r="G6" s="49">
+        <f>G4*G5</f>
+        <v>10</v>
+      </c>
+      <c r="H6" s="107" t="s">
+        <v>91</v>
+      </c>
+      <c r="L6" s="108" t="s">
+        <v>134</v>
+      </c>
+      <c r="M6" s="105"/>
+      <c r="N6" s="50">
+        <v>10</v>
+      </c>
+      <c r="O6" s="123" t="s">
+        <v>141</v>
+      </c>
+      <c r="P6" s="118">
+        <f>IF(O6="ON",N6,0)</f>
+        <v>10</v>
+      </c>
+      <c r="Q6" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="R6" s="109">
+        <f>IF(Q6="ON",N6,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C7" s="84" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="47">
         <v>8</v>
       </c>
       <c r="F7" s="61">
         <v>8</v>
       </c>
-      <c r="G7" s="50" t="s">
+      <c r="G7" s="61">
+        <v>8</v>
+      </c>
+      <c r="H7" s="161" t="s">
+        <v>88</v>
+      </c>
+      <c r="L7" s="110" t="s">
+        <v>135</v>
+      </c>
+      <c r="M7" s="111"/>
+      <c r="N7" s="51">
+        <v>7</v>
+      </c>
+      <c r="O7" s="124" t="s">
+        <v>141</v>
+      </c>
+      <c r="P7" s="119">
+        <f t="shared" ref="P7:P11" si="0">IF(O7="ON",N7,0)</f>
+        <v>7</v>
+      </c>
+      <c r="Q7" s="128" t="s">
+        <v>141</v>
+      </c>
+      <c r="R7" s="112">
+        <f t="shared" ref="R7:R11" si="1">IF(Q7="ON",N7,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="86"/>
+      <c r="D8" s="49" t="s">
         <v>89</v>
-      </c>
-      <c r="J7" s="55" t="s">
-        <v>112</v>
-      </c>
-      <c r="K7" s="48">
-        <f>K5*K6/100*1000</f>
-        <v>400</v>
-      </c>
-      <c r="L7" s="48">
-        <f>L5*L6/100*1000</f>
-        <v>800</v>
-      </c>
-      <c r="M7" s="48">
-        <f>M5*M6/100*1000</f>
-        <v>1200</v>
-      </c>
-      <c r="N7" s="48">
-        <f>N5*N6/100*1000</f>
-        <v>1600</v>
-      </c>
-      <c r="O7" s="48">
-        <f>O5*O6/100*1000</f>
-        <v>2000</v>
-      </c>
-      <c r="P7" s="51" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="74"/>
-      <c r="C8" s="49" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="49">
-        <f>D6/D7</f>
-        <v>1</v>
       </c>
       <c r="E8" s="49">
         <f>E6/E7</f>
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="F8" s="49">
         <f>F6/F7</f>
         <v>1.25</v>
       </c>
-      <c r="G8" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="J8" s="56" t="s">
-        <v>109</v>
-      </c>
-      <c r="K8" s="49">
-        <f>$K4/K7</f>
-        <v>2.5</v>
-      </c>
-      <c r="L8" s="49">
-        <f t="shared" ref="L8:O8" si="0">$K4/L7</f>
+      <c r="G8" s="49">
+        <f>G6/G7</f>
         <v>1.25</v>
       </c>
-      <c r="M8" s="49">
+      <c r="H8" s="107" t="s">
+        <v>90</v>
+      </c>
+      <c r="L8" s="110" t="s">
+        <v>136</v>
+      </c>
+      <c r="M8" s="111"/>
+      <c r="N8" s="51">
+        <v>7</v>
+      </c>
+      <c r="O8" s="125" t="s">
+        <v>142</v>
+      </c>
+      <c r="P8" s="120">
         <f t="shared" si="0"/>
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="N8" s="49">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="128" t="s">
+        <v>141</v>
+      </c>
+      <c r="R8" s="112">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C9" s="84" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="47">
+        <v>125</v>
+      </c>
+      <c r="F9" s="61">
+        <v>392</v>
+      </c>
+      <c r="G9" s="61">
+        <v>350</v>
+      </c>
+      <c r="H9" s="161"/>
+      <c r="L9" s="110" t="s">
+        <v>137</v>
+      </c>
+      <c r="M9" s="111"/>
+      <c r="N9" s="51">
+        <v>18</v>
+      </c>
+      <c r="O9" s="124" t="s">
+        <v>141</v>
+      </c>
+      <c r="P9" s="119">
         <f t="shared" si="0"/>
-        <v>0.625</v>
-      </c>
-      <c r="O8" s="49">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="P8" s="52" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="72" t="s">
-        <v>103</v>
-      </c>
-      <c r="C9" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q9" s="128" t="s">
+        <v>141</v>
+      </c>
+      <c r="R9" s="112">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C10" s="85"/>
+      <c r="D10" s="48" t="s">
         <v>93</v>
-      </c>
-      <c r="D9" s="47">
-        <v>125</v>
-      </c>
-      <c r="E9" s="61">
-        <v>392</v>
-      </c>
-      <c r="F9" s="61">
-        <v>350</v>
-      </c>
-      <c r="G9" s="50"/>
-    </row>
-    <row r="10" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="73"/>
-      <c r="C10" s="48" t="s">
-        <v>94</v>
-      </c>
-      <c r="D10" s="48">
-        <f>D7*D9</f>
-        <v>1000</v>
       </c>
       <c r="E10" s="48">
         <f>E7*E9</f>
-        <v>3136</v>
+        <v>1000</v>
       </c>
       <c r="F10" s="48">
         <f>F7*F9</f>
+        <v>3136</v>
+      </c>
+      <c r="G10" s="48">
+        <f>G7*G9</f>
         <v>2800</v>
       </c>
-      <c r="G10" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="J10" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="K10" s="59">
-        <v>2000</v>
-      </c>
-      <c r="L10" s="60" t="s">
-        <v>108</v>
-      </c>
-      <c r="M10" s="45"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="45"/>
-      <c r="P10" s="45"/>
-    </row>
-    <row r="11" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="74"/>
-      <c r="C11" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="49">
-        <f>D6/D10</f>
-        <v>8.0000000000000002E-3</v>
+      <c r="H10" s="162" t="s">
+        <v>88</v>
+      </c>
+      <c r="L10" s="110" t="s">
+        <v>138</v>
+      </c>
+      <c r="M10" s="111"/>
+      <c r="N10" s="51">
+        <v>2500</v>
+      </c>
+      <c r="O10" s="125" t="s">
+        <v>142</v>
+      </c>
+      <c r="P10" s="120">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="128" t="s">
+        <v>141</v>
+      </c>
+      <c r="R10" s="112">
+        <f t="shared" si="1"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="86"/>
+      <c r="D11" s="49" t="s">
+        <v>94</v>
       </c>
       <c r="E11" s="49">
         <f>E6/E10</f>
-        <v>3.1887755102040817E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F11" s="49">
         <f>F6/F10</f>
+        <v>3.1887755102040817E-3</v>
+      </c>
+      <c r="G11" s="49">
+        <f>G6/G10</f>
         <v>3.5714285714285713E-3</v>
       </c>
-      <c r="G11" s="52" t="s">
-        <v>92</v>
-      </c>
-      <c r="J11" s="57" t="s">
+      <c r="H11" s="107" t="s">
+        <v>91</v>
+      </c>
+      <c r="L11" s="113" t="s">
+        <v>139</v>
+      </c>
+      <c r="M11" s="114"/>
+      <c r="N11" s="52">
+        <v>80</v>
+      </c>
+      <c r="O11" s="126" t="s">
+        <v>142</v>
+      </c>
+      <c r="P11" s="121">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="R11" s="115">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L12" s="46"/>
+      <c r="M12" s="46"/>
+      <c r="O12" s="116" t="s">
+        <v>152</v>
+      </c>
+      <c r="P12" s="122">
+        <f>SUM(P6:P11)</f>
+        <v>35</v>
+      </c>
+      <c r="Q12" s="116" t="s">
+        <v>152</v>
+      </c>
+      <c r="R12" s="117">
+        <f>SUM(R6:R11)</f>
+        <v>2622</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="46"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="L13" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="M13" s="46"/>
+    </row>
+    <row r="14" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="58" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="59">
+        <v>1000</v>
+      </c>
+      <c r="E14" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="L14" s="133" t="s">
+        <v>140</v>
+      </c>
+      <c r="M14" s="134"/>
+      <c r="N14" s="145">
+        <f>P12</f>
+        <v>35</v>
+      </c>
+      <c r="O14" s="161" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="47">
+        <v>2</v>
+      </c>
+      <c r="E15" s="47">
+        <v>2</v>
+      </c>
+      <c r="F15" s="47">
+        <v>2</v>
+      </c>
+      <c r="G15" s="47">
+        <v>2</v>
+      </c>
+      <c r="H15" s="47">
+        <v>2</v>
+      </c>
+      <c r="I15" s="161" t="s">
         <v>98</v>
       </c>
-      <c r="K11" s="53">
+      <c r="L15" s="149" t="s">
+        <v>143</v>
+      </c>
+      <c r="M15" s="150"/>
+      <c r="N15" s="159">
+        <f>R12</f>
+        <v>2622</v>
+      </c>
+      <c r="O15" s="107" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C16" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="48">
+        <v>20</v>
+      </c>
+      <c r="E16" s="48">
+        <v>40</v>
+      </c>
+      <c r="F16" s="48">
+        <v>60</v>
+      </c>
+      <c r="G16" s="48">
+        <v>80</v>
+      </c>
+      <c r="H16" s="48">
+        <v>100</v>
+      </c>
+      <c r="I16" s="162" t="s">
+        <v>106</v>
+      </c>
+      <c r="L16" s="46"/>
+      <c r="M16" s="46"/>
+    </row>
+    <row r="17" spans="3:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="48">
+        <f>D15*D16/100*1000</f>
+        <v>400</v>
+      </c>
+      <c r="E17" s="48">
+        <f>E15*E16/100*1000</f>
+        <v>800</v>
+      </c>
+      <c r="F17" s="48">
+        <f>F15*F16/100*1000</f>
+        <v>1200</v>
+      </c>
+      <c r="G17" s="48">
+        <f>G15*G16/100*1000</f>
+        <v>1600</v>
+      </c>
+      <c r="H17" s="48">
+        <f>H15*H16/100*1000</f>
+        <v>2000</v>
+      </c>
+      <c r="I17" s="162" t="s">
+        <v>110</v>
+      </c>
+      <c r="L17" s="46" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="3:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="49">
+        <f>$D14/D17</f>
+        <v>2.5</v>
+      </c>
+      <c r="E18" s="49">
+        <f>$D14/E17</f>
+        <v>1.25</v>
+      </c>
+      <c r="F18" s="49">
+        <f>$D14/F17</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G18" s="49">
+        <f>$D14/G17</f>
+        <v>0.625</v>
+      </c>
+      <c r="H18" s="49">
+        <f>$D14/H17</f>
+        <v>0.5</v>
+      </c>
+      <c r="I18" s="107" t="s">
+        <v>109</v>
+      </c>
+      <c r="L18" s="133" t="s">
+        <v>146</v>
+      </c>
+      <c r="M18" s="134"/>
+      <c r="N18" s="157">
+        <v>1500</v>
+      </c>
+      <c r="O18" s="164">
+        <v>2000</v>
+      </c>
+      <c r="P18" s="158">
+        <v>2500</v>
+      </c>
+      <c r="Q18" s="163" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="3:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="46"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="I19" s="2"/>
+      <c r="L19" s="151" t="s">
+        <v>140</v>
+      </c>
+      <c r="M19" s="152"/>
+      <c r="N19" s="146">
+        <f>N$18/$N$14</f>
+        <v>42.857142857142854</v>
+      </c>
+      <c r="O19" s="69">
+        <f>O$18/$N$14</f>
+        <v>57.142857142857146</v>
+      </c>
+      <c r="P19" s="69">
+        <f>P$18/$N$14</f>
+        <v>71.428571428571431</v>
+      </c>
+      <c r="Q19" s="162" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="3:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="58" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="59">
+        <v>2000</v>
+      </c>
+      <c r="E20" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="H20" s="45"/>
+      <c r="I20" s="2"/>
+      <c r="L20" s="153" t="s">
+        <v>151</v>
+      </c>
+      <c r="M20" s="154">
+        <v>20</v>
+      </c>
+      <c r="N20" s="147">
+        <f>N$18/($N$15*$M20/100)*60</f>
+        <v>171.62471395881008</v>
+      </c>
+      <c r="O20" s="143">
+        <f>O$18/($N$15*$M20/100)*60</f>
+        <v>228.83295194508011</v>
+      </c>
+      <c r="P20" s="143">
+        <f>P$18/($N$15*$M20/100)*60</f>
+        <v>286.04118993135012</v>
+      </c>
+      <c r="Q20" s="162" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C21" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="53">
         <v>2</v>
       </c>
-      <c r="L11" s="53">
+      <c r="E21" s="53">
         <v>2</v>
       </c>
-      <c r="M11" s="47">
+      <c r="F21" s="47">
         <v>2</v>
       </c>
-      <c r="N11" s="47">
+      <c r="G21" s="47">
         <v>2</v>
       </c>
-      <c r="O11" s="47">
+      <c r="H21" s="47">
         <v>2</v>
       </c>
-      <c r="P11" s="50" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="J12" s="55" t="s">
+      <c r="I21" s="161" t="s">
+        <v>98</v>
+      </c>
+      <c r="L21" s="85"/>
+      <c r="M21" s="154">
+        <v>40</v>
+      </c>
+      <c r="N21" s="147">
+        <f>N$18/($N$15*$M21/100)*60</f>
+        <v>85.812356979405038</v>
+      </c>
+      <c r="O21" s="143">
+        <f>O$18/($N$15*$M21/100)*60</f>
+        <v>114.41647597254006</v>
+      </c>
+      <c r="P21" s="143">
+        <f>P$18/($N$15*$M21/100)*60</f>
+        <v>143.02059496567506</v>
+      </c>
+      <c r="Q21" s="162" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C22" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="48">
+        <v>20</v>
+      </c>
+      <c r="E22" s="48">
+        <v>40</v>
+      </c>
+      <c r="F22" s="48">
+        <v>60</v>
+      </c>
+      <c r="G22" s="48">
+        <v>80</v>
+      </c>
+      <c r="H22" s="48">
+        <v>100</v>
+      </c>
+      <c r="I22" s="162" t="s">
         <v>106</v>
       </c>
-      <c r="K12" s="48">
+      <c r="L22" s="85"/>
+      <c r="M22" s="154">
+        <v>60</v>
+      </c>
+      <c r="N22" s="147">
+        <f>N$18/($N$15*$M22/100)*60</f>
+        <v>57.208237986270021</v>
+      </c>
+      <c r="O22" s="143">
+        <f>O$18/($N$15*$M22/100)*60</f>
+        <v>76.277650648360023</v>
+      </c>
+      <c r="P22" s="143">
+        <f>P$18/($N$15*$M22/100)*60</f>
+        <v>95.347063310450039</v>
+      </c>
+      <c r="Q22" s="162" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C23" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="48">
+        <f>D21*D22/100*1000</f>
+        <v>400</v>
+      </c>
+      <c r="E23" s="48">
+        <f>E21*E22/100*1000</f>
+        <v>800</v>
+      </c>
+      <c r="F23" s="48">
+        <f>F21*F22/100*1000</f>
+        <v>1200</v>
+      </c>
+      <c r="G23" s="48">
+        <f>G21*G22/100*1000</f>
+        <v>1600</v>
+      </c>
+      <c r="H23" s="48">
+        <f>H21*H22/100*1000</f>
+        <v>2000</v>
+      </c>
+      <c r="I23" s="162" t="s">
+        <v>110</v>
+      </c>
+      <c r="L23" s="85"/>
+      <c r="M23" s="154">
+        <v>80</v>
+      </c>
+      <c r="N23" s="147">
+        <f>N$18/($N$15*$M23/100)*60</f>
+        <v>42.906178489702519</v>
+      </c>
+      <c r="O23" s="143">
+        <f>O$18/($N$15*$M23/100)*60</f>
+        <v>57.208237986270028</v>
+      </c>
+      <c r="P23" s="143">
+        <f>P$18/($N$15*$M23/100)*60</f>
+        <v>71.51029748283753</v>
+      </c>
+      <c r="Q23" s="162" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="3:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="49">
+        <f>$D20/D23</f>
+        <v>5</v>
+      </c>
+      <c r="E24" s="49">
+        <f>$D20/E23</f>
+        <v>2.5</v>
+      </c>
+      <c r="F24" s="49">
+        <f>$D20/F23</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="G24" s="49">
+        <f>$D20/G23</f>
+        <v>1.25</v>
+      </c>
+      <c r="H24" s="49">
+        <f>$D20/H23</f>
+        <v>1</v>
+      </c>
+      <c r="I24" s="107" t="s">
+        <v>109</v>
+      </c>
+      <c r="L24" s="86"/>
+      <c r="M24" s="155">
+        <v>100</v>
+      </c>
+      <c r="N24" s="148">
+        <f>N$18/($N$15*$M24/100)*60</f>
+        <v>34.32494279176202</v>
+      </c>
+      <c r="O24" s="144">
+        <f>O$18/($N$15*$M24/100)*60</f>
+        <v>45.766590389016017</v>
+      </c>
+      <c r="P24" s="144">
+        <f>P$18/($N$15*$M24/100)*60</f>
+        <v>57.208237986270028</v>
+      </c>
+      <c r="Q24" s="107" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="3:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="46"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="3:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="58" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="59">
+        <v>2000</v>
+      </c>
+      <c r="E26" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="H26" s="45"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C27" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" s="47">
+        <v>2.6219999999999999</v>
+      </c>
+      <c r="E27" s="47">
+        <v>2.6219999999999999</v>
+      </c>
+      <c r="F27" s="47">
+        <v>2.6219999999999999</v>
+      </c>
+      <c r="G27" s="47">
+        <v>2.6219999999999999</v>
+      </c>
+      <c r="H27" s="47">
+        <v>2.6219999999999999</v>
+      </c>
+      <c r="I27" s="161" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C28" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" s="48">
         <v>20</v>
       </c>
-      <c r="L12" s="48">
+      <c r="E28" s="48">
         <v>40</v>
       </c>
-      <c r="M12" s="48">
+      <c r="F28" s="48">
         <v>60</v>
       </c>
-      <c r="N12" s="48">
+      <c r="G28" s="48">
         <v>80</v>
       </c>
-      <c r="O12" s="48">
+      <c r="H28" s="48">
         <v>100</v>
       </c>
-      <c r="P12" s="51" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="J13" s="55" t="s">
-        <v>112</v>
-      </c>
-      <c r="K13" s="48">
-        <f>K11*K12/100*1000</f>
-        <v>400</v>
-      </c>
-      <c r="L13" s="48">
-        <f>L11*L12/100*1000</f>
-        <v>800</v>
-      </c>
-      <c r="M13" s="48">
-        <f>M11*M12/100*1000</f>
-        <v>1200</v>
-      </c>
-      <c r="N13" s="48">
-        <f>N11*N12/100*1000</f>
-        <v>1600</v>
-      </c>
-      <c r="O13" s="48">
-        <f>O11*O12/100*1000</f>
-        <v>2000</v>
-      </c>
-      <c r="P13" s="51" t="s">
+      <c r="I28" s="162" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C29" s="55" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="14" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J14" s="56" t="s">
+      <c r="D29" s="48">
+        <f>D27*D28/100*1000</f>
+        <v>524.4</v>
+      </c>
+      <c r="E29" s="48">
+        <f>E27*E28/100*1000</f>
+        <v>1048.8</v>
+      </c>
+      <c r="F29" s="48">
+        <f>F27*F28/100*1000</f>
+        <v>1573.1999999999998</v>
+      </c>
+      <c r="G29" s="48">
+        <f>G27*G28/100*1000</f>
+        <v>2097.6</v>
+      </c>
+      <c r="H29" s="48">
+        <f>H27*H28/100*1000</f>
+        <v>2622</v>
+      </c>
+      <c r="I29" s="162" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="3:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" s="160">
+        <f>$D26/D29</f>
+        <v>3.8138825324180017</v>
+      </c>
+      <c r="E30" s="160">
+        <f>$D26/E29</f>
+        <v>1.9069412662090008</v>
+      </c>
+      <c r="F30" s="160">
+        <f>$D26/F29</f>
+        <v>1.2712941774726674</v>
+      </c>
+      <c r="G30" s="160">
+        <f>$D26/G29</f>
+        <v>0.95347063310450042</v>
+      </c>
+      <c r="H30" s="160">
+        <f>$D26/H29</f>
+        <v>0.76277650648360029</v>
+      </c>
+      <c r="I30" s="107" t="s">
         <v>109</v>
       </c>
-      <c r="K14" s="49">
-        <f>$K10/K13</f>
-        <v>5</v>
-      </c>
-      <c r="L14" s="49">
-        <f t="shared" ref="L14" si="1">$K10/L13</f>
-        <v>2.5</v>
-      </c>
-      <c r="M14" s="49">
-        <f t="shared" ref="M14" si="2">$K10/M13</f>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="N14" s="49">
-        <f t="shared" ref="N14" si="3">$K10/N13</f>
-        <v>1.25</v>
-      </c>
-      <c r="O14" s="49">
-        <f t="shared" ref="O14" si="4">$K10/O13</f>
-        <v>1</v>
-      </c>
-      <c r="P14" s="52" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J16" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="K16" s="59">
-        <v>2000</v>
-      </c>
-      <c r="L16" s="60" t="s">
+    </row>
+    <row r="31" spans="3:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="M16" s="45"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="45"/>
-    </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="J17" s="54" t="s">
-        <v>98</v>
-      </c>
-      <c r="K17" s="47">
-        <v>2.5</v>
-      </c>
-      <c r="L17" s="47">
-        <v>2.5</v>
-      </c>
-      <c r="M17" s="47">
-        <v>2.5</v>
-      </c>
-      <c r="N17" s="47">
-        <v>2.5</v>
-      </c>
-      <c r="O17" s="47">
-        <v>2.5</v>
-      </c>
-      <c r="P17" s="50" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C18">
-        <v>280</v>
-      </c>
-      <c r="D18" s="45">
-        <v>250</v>
-      </c>
-      <c r="J18" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="K18" s="48">
-        <v>20</v>
-      </c>
-      <c r="L18" s="48">
-        <v>40</v>
-      </c>
-      <c r="M18" s="48">
-        <v>60</v>
-      </c>
-      <c r="N18" s="48">
-        <v>80</v>
-      </c>
-      <c r="O18" s="48">
-        <v>100</v>
-      </c>
-      <c r="P18" s="51" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C19">
-        <v>7</v>
-      </c>
-      <c r="D19" s="45">
-        <v>7</v>
-      </c>
-      <c r="J19" s="55" t="s">
-        <v>112</v>
-      </c>
-      <c r="K19" s="48">
-        <f>K17*K18/100*1000</f>
-        <v>500</v>
-      </c>
-      <c r="L19" s="48">
-        <f>L17*L18/100*1000</f>
-        <v>1000</v>
-      </c>
-      <c r="M19" s="48">
-        <f>M17*M18/100*1000</f>
-        <v>1500</v>
-      </c>
-      <c r="N19" s="48">
-        <f>N17*N18/100*1000</f>
-        <v>2000</v>
-      </c>
-      <c r="O19" s="48">
-        <f>O17*O18/100*1000</f>
-        <v>2500</v>
-      </c>
-      <c r="P19" s="51" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="3:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20">
-        <f>C18*C19</f>
-        <v>1960</v>
-      </c>
-      <c r="D20" s="45">
-        <f>D18*D19</f>
-        <v>1750</v>
-      </c>
-      <c r="J20" s="56" t="s">
-        <v>109</v>
-      </c>
-      <c r="K20" s="49">
-        <f>$K16/K19</f>
-        <v>4</v>
-      </c>
-      <c r="L20" s="49">
-        <f t="shared" ref="L20" si="5">$K16/L19</f>
-        <v>2</v>
-      </c>
-      <c r="M20" s="49">
-        <f t="shared" ref="M20" si="6">$K16/M19</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="N20" s="49">
-        <f t="shared" ref="N20" si="7">$K16/N19</f>
-        <v>1</v>
-      </c>
-      <c r="O20" s="49">
-        <f t="shared" ref="O20" si="8">$K16/O19</f>
-        <v>0.8</v>
-      </c>
-      <c r="P20" s="52" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="C21">
-        <f>C20/5</f>
-        <v>392</v>
-      </c>
-      <c r="D21" s="45">
-        <f>D20/5</f>
-        <v>350</v>
-      </c>
-    </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="D22" s="45"/>
+      <c r="D31" s="144">
+        <f>D30*60</f>
+        <v>228.83295194508011</v>
+      </c>
+      <c r="E31" s="144">
+        <f t="shared" ref="E31:H31" si="2">E30*60</f>
+        <v>114.41647597254006</v>
+      </c>
+      <c r="F31" s="144">
+        <f t="shared" si="2"/>
+        <v>76.277650648360037</v>
+      </c>
+      <c r="G31" s="144">
+        <f t="shared" si="2"/>
+        <v>57.208237986270028</v>
+      </c>
+      <c r="H31" s="144">
+        <f t="shared" si="2"/>
+        <v>45.766590389016017</v>
+      </c>
+      <c r="I31" s="107" t="s">
+        <v>150</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B4:B6"/>
+  <mergeCells count="18">
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="L20:L24"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="L4:M5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3677,94 +4800,130 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.125" style="45" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" customWidth="1"/>
+    <col min="6" max="6" width="9.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="165"/>
+      <c r="C3" s="142" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="142" t="s">
+        <v>158</v>
+      </c>
+      <c r="E3" s="105" t="s">
+        <v>159</v>
+      </c>
+      <c r="F3" s="105"/>
+      <c r="G3" s="50"/>
+    </row>
+    <row r="4" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="166"/>
+      <c r="C4" s="106" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="106" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="106" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" s="106" t="s">
+        <v>119</v>
+      </c>
+      <c r="G4" s="52"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="167" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="47">
+        <v>3.3</v>
+      </c>
+      <c r="D5" s="47">
+        <v>3.3</v>
+      </c>
+      <c r="E5" s="47">
+        <v>3.3</v>
+      </c>
+      <c r="F5" s="47">
+        <v>3.3</v>
+      </c>
+      <c r="G5" s="109" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="168" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="48">
+        <v>430</v>
+      </c>
+      <c r="D6" s="48">
+        <v>470</v>
+      </c>
+      <c r="E6" s="48">
+        <v>470</v>
+      </c>
+      <c r="F6" s="48">
+        <v>180</v>
+      </c>
+      <c r="G6" s="169" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="127" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="170">
+        <f>C5/C6*1000</f>
+        <v>7.6744186046511622</v>
+      </c>
+      <c r="D7" s="170">
+        <f>D5/D6*1000</f>
+        <v>7.0212765957446797</v>
+      </c>
+      <c r="E7" s="170">
+        <f>E5/E6*1000</f>
+        <v>7.0212765957446797</v>
+      </c>
+      <c r="F7" s="170">
+        <f>F5/F6*1000</f>
+        <v>18.333333333333332</v>
+      </c>
+      <c r="G7" s="115" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E3:F3"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:E7"/>
+  <dimension ref="B2:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="7.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C5">
-        <v>3.3</v>
-      </c>
-      <c r="D5" s="45">
-        <v>3.3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6">
-        <v>470</v>
-      </c>
-      <c r="D6" s="45">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="63">
-        <f>C5/C6*1000</f>
-        <v>7.0212765957446797</v>
-      </c>
-      <c r="D7" s="63">
-        <f>D5/D6*1000</f>
-        <v>18.333333333333332</v>
-      </c>
-      <c r="E7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F28"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3777,290 +4936,290 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D4" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="2:6" s="45" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="46" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="75" t="s">
-        <v>129</v>
-      </c>
-      <c r="D7" s="76" t="s">
-        <v>128</v>
-      </c>
-      <c r="E7" s="76" t="s">
+      <c r="C7" s="63" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="64" t="s">
         <v>125</v>
       </c>
-      <c r="F7" s="77"/>
+      <c r="E7" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" s="65"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C8" s="78">
+      <c r="C8" s="66">
         <v>5</v>
       </c>
-      <c r="D8" s="79">
+      <c r="D8" s="67">
         <v>0.11</v>
       </c>
       <c r="E8" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="50"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C9" s="68">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D9" s="69">
+        <v>0.11</v>
+      </c>
+      <c r="E9" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="51"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C10" s="68">
+        <v>4.8</v>
+      </c>
+      <c r="D10" s="69">
+        <v>0.11</v>
+      </c>
+      <c r="E10" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" s="51"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C11" s="68">
+        <v>4.7</v>
+      </c>
+      <c r="D11" s="69">
+        <v>0.11</v>
+      </c>
+      <c r="E11" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" s="51"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C12" s="68">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D12" s="69">
+        <v>0.11</v>
+      </c>
+      <c r="E12" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12" s="51"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="68">
+        <v>4.5</v>
+      </c>
+      <c r="D13" s="69">
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" s="51"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C14" s="68">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D14" s="69">
+        <v>0.1</v>
+      </c>
+      <c r="E14" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="F14" s="51"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="68">
+        <v>4.3</v>
+      </c>
+      <c r="D15" s="69">
+        <v>0.09</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="F15" s="51"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="70">
+        <v>4.2</v>
+      </c>
+      <c r="D16" s="71">
+        <v>0.09</v>
+      </c>
+      <c r="E16" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="F16" s="73"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="70">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D17" s="71">
+        <v>0.09</v>
+      </c>
+      <c r="E17" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="F17" s="73"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="70">
+        <v>4</v>
+      </c>
+      <c r="D18" s="71">
+        <v>0.09</v>
+      </c>
+      <c r="E18" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" s="73"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="70">
+        <v>3.9</v>
+      </c>
+      <c r="D19" s="71">
+        <v>0.08</v>
+      </c>
+      <c r="E19" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="F19" s="73"/>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C20" s="70">
+        <v>3.8</v>
+      </c>
+      <c r="D20" s="71">
+        <v>0.08</v>
+      </c>
+      <c r="E20" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="F20" s="73"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="70">
+        <v>3.7</v>
+      </c>
+      <c r="D21" s="71">
+        <v>0.08</v>
+      </c>
+      <c r="E21" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="F21" s="73"/>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C22" s="70">
+        <v>3.6</v>
+      </c>
+      <c r="D22" s="71">
+        <v>0.08</v>
+      </c>
+      <c r="E22" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="F22" s="73"/>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C23" s="70">
+        <v>3.5</v>
+      </c>
+      <c r="D23" s="71">
+        <v>0.08</v>
+      </c>
+      <c r="E23" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="F23" s="73"/>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C24" s="70">
+        <v>3.4</v>
+      </c>
+      <c r="D24" s="71">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E24" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" s="73"/>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C25" s="68">
+        <v>3.3</v>
+      </c>
+      <c r="D25" s="69">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E25" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="F25" s="51"/>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C26" s="68">
+        <v>3.2</v>
+      </c>
+      <c r="D26" s="69">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E26" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="F26" s="51"/>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C27" s="68">
+        <v>3.1</v>
+      </c>
+      <c r="D27" s="69">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E27" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="F27" s="51" t="s">
         <v>124</v>
       </c>
-      <c r="F8" s="50"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="80">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="D9" s="81">
-        <v>0.11</v>
-      </c>
-      <c r="E9" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="F9" s="51"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="80">
-        <v>4.8</v>
-      </c>
-      <c r="D10" s="81">
-        <v>0.11</v>
-      </c>
-      <c r="E10" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="F10" s="51"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C11" s="80">
-        <v>4.7</v>
-      </c>
-      <c r="D11" s="81">
-        <v>0.11</v>
-      </c>
-      <c r="E11" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="F11" s="51"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C12" s="80">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="D12" s="81">
-        <v>0.11</v>
-      </c>
-      <c r="E12" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="F12" s="51"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="80">
-        <v>4.5</v>
-      </c>
-      <c r="D13" s="81">
-        <v>0.1</v>
-      </c>
-      <c r="E13" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="F13" s="51"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="80">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D14" s="81">
-        <v>0.1</v>
-      </c>
-      <c r="E14" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="F14" s="51"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="80">
-        <v>4.3</v>
-      </c>
-      <c r="D15" s="81">
-        <v>0.09</v>
-      </c>
-      <c r="E15" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="F15" s="51"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C16" s="82">
-        <v>4.2</v>
-      </c>
-      <c r="D16" s="83">
-        <v>0.09</v>
-      </c>
-      <c r="E16" s="84" t="s">
-        <v>124</v>
-      </c>
-      <c r="F16" s="85"/>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="82">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D17" s="83">
-        <v>0.09</v>
-      </c>
-      <c r="E17" s="84" t="s">
-        <v>124</v>
-      </c>
-      <c r="F17" s="85"/>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C18" s="82">
-        <v>4</v>
-      </c>
-      <c r="D18" s="83">
-        <v>0.09</v>
-      </c>
-      <c r="E18" s="84" t="s">
-        <v>124</v>
-      </c>
-      <c r="F18" s="85"/>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C19" s="82">
-        <v>3.9</v>
-      </c>
-      <c r="D19" s="83">
-        <v>0.08</v>
-      </c>
-      <c r="E19" s="84" t="s">
-        <v>124</v>
-      </c>
-      <c r="F19" s="85"/>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C20" s="82">
-        <v>3.8</v>
-      </c>
-      <c r="D20" s="83">
-        <v>0.08</v>
-      </c>
-      <c r="E20" s="84" t="s">
-        <v>124</v>
-      </c>
-      <c r="F20" s="85"/>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C21" s="82">
-        <v>3.7</v>
-      </c>
-      <c r="D21" s="83">
-        <v>0.08</v>
-      </c>
-      <c r="E21" s="84" t="s">
-        <v>124</v>
-      </c>
-      <c r="F21" s="85"/>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C22" s="82">
-        <v>3.6</v>
-      </c>
-      <c r="D22" s="83">
-        <v>0.08</v>
-      </c>
-      <c r="E22" s="84" t="s">
-        <v>124</v>
-      </c>
-      <c r="F22" s="85"/>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C23" s="82">
-        <v>3.5</v>
-      </c>
-      <c r="D23" s="83">
-        <v>0.08</v>
-      </c>
-      <c r="E23" s="84" t="s">
-        <v>124</v>
-      </c>
-      <c r="F23" s="85"/>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C24" s="82">
-        <v>3.4</v>
-      </c>
-      <c r="D24" s="83">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E24" s="84" t="s">
-        <v>124</v>
-      </c>
-      <c r="F24" s="85"/>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C25" s="80">
-        <v>3.3</v>
-      </c>
-      <c r="D25" s="81">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E25" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="F25" s="51"/>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C26" s="80">
-        <v>3.2</v>
-      </c>
-      <c r="D26" s="81">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E26" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="F26" s="51"/>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C27" s="80">
-        <v>3.1</v>
-      </c>
-      <c r="D27" s="81">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E27" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="F27" s="51" t="s">
-        <v>127</v>
-      </c>
     </row>
     <row r="28" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C28" s="86">
+      <c r="C28" s="74">
         <v>3</v>
       </c>
-      <c r="D28" s="87">
+      <c r="D28" s="75">
         <v>0.06</v>
       </c>
       <c r="E28" s="49" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F28" s="52"/>
     </row>
@@ -4068,4 +5227,188 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="D16:E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="171" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="C3" s="103" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" s="103"/>
+      <c r="E3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F3" s="173" t="s">
+        <v>163</v>
+      </c>
+      <c r="G3" s="173"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="174" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" s="172" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" s="172" t="s">
+        <v>164</v>
+      </c>
+      <c r="G4" s="172" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="1">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>66.790000000000006</v>
+      </c>
+      <c r="D5">
+        <f>C5/10000</f>
+        <v>6.6790000000000009E-3</v>
+      </c>
+      <c r="E5" s="104">
+        <f>D5*2.5</f>
+        <v>1.6697500000000004E-2</v>
+      </c>
+      <c r="F5">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="1">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>84.22</v>
+      </c>
+      <c r="D6" s="45">
+        <f>C6/10000</f>
+        <v>8.4220000000000007E-3</v>
+      </c>
+      <c r="E6" s="104">
+        <f>D6*2.5</f>
+        <v>2.1055000000000001E-2</v>
+      </c>
+      <c r="F6">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>106.2</v>
+      </c>
+      <c r="D7" s="45">
+        <f>C7/10000</f>
+        <v>1.0620000000000001E-2</v>
+      </c>
+      <c r="E7" s="104">
+        <f>D7*2.5</f>
+        <v>2.6550000000000004E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.47699999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
+        <v>26</v>
+      </c>
+      <c r="C8">
+        <v>133.9</v>
+      </c>
+      <c r="D8" s="45">
+        <f>C8/10000</f>
+        <v>1.3390000000000001E-2</v>
+      </c>
+      <c r="E8" s="104">
+        <f>D8*2.5</f>
+        <v>3.3475000000000005E-2</v>
+      </c>
+      <c r="F8">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="G8">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>168.9</v>
+      </c>
+      <c r="D9" s="45">
+        <f>C9/10000</f>
+        <v>1.6890000000000002E-2</v>
+      </c>
+      <c r="E9" s="104">
+        <f>D9*2.5</f>
+        <v>4.2225000000000006E-2</v>
+      </c>
+      <c r="F9">
+        <v>0.28799999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
+        <v>28</v>
+      </c>
+      <c r="C10">
+        <v>212.9</v>
+      </c>
+      <c r="D10" s="45">
+        <f>C10/10000</f>
+        <v>2.129E-2</v>
+      </c>
+      <c r="E10" s="104">
+        <f>D10*2.5</f>
+        <v>5.3225000000000001E-2</v>
+      </c>
+      <c r="F10">
+        <v>0.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C3:D3"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Pipette] S/V 압력 Test update
</commit_message>
<xml_diff>
--- a/1_Plasma_Pipette/4_Review data/Plasma_Pipette Review Data.xlsx
+++ b/1_Plasma_Pipette/4_Review data/Plasma_Pipette Review Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="하네스" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="203">
   <si>
     <t>Battery 용량</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -819,6 +819,22 @@
   </si>
   <si>
     <t>장시간 Test 후 dead - 출력이 낮게 나옴</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Measure</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Press[MPa]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Press Test @ Vcc=4V</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma 동작범위</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1917,7 +1933,7 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2180,135 +2196,6 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2340,6 +2227,147 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="35" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="20" fillId="35" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="20" fillId="35" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="20% - 강조색1" xfId="17" builtinId="30" customBuiltin="1"/>
@@ -2471,7 +2499,7 @@
       <xdr:col>22</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2868,7 +2896,7 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="140" t="s">
+      <c r="B4" s="156" t="s">
         <v>131</v>
       </c>
       <c r="C4" s="76">
@@ -2877,7 +2905,7 @@
       <c r="D4" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="132" t="s">
+      <c r="E4" s="150" t="s">
         <v>26</v>
       </c>
       <c r="F4" s="36">
@@ -2900,21 +2928,21 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="141"/>
+      <c r="B5" s="157"/>
       <c r="C5" s="78">
         <v>2</v>
       </c>
       <c r="D5" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="133"/>
+      <c r="E5" s="148"/>
       <c r="F5" s="32">
         <v>2</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="138" t="s">
+      <c r="I5" s="154" t="s">
         <v>48</v>
       </c>
       <c r="J5" s="38" t="s">
@@ -2928,21 +2956,21 @@
       </c>
     </row>
     <row r="6" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="142"/>
+      <c r="B6" s="158"/>
       <c r="C6" s="80">
         <v>3</v>
       </c>
       <c r="D6" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="134"/>
+      <c r="E6" s="149"/>
       <c r="F6" s="19">
         <v>3</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I6" s="138"/>
+      <c r="I6" s="154"/>
       <c r="J6" s="42" t="s">
         <v>55</v>
       </c>
@@ -2954,7 +2982,7 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I7" s="138"/>
+      <c r="I7" s="154"/>
       <c r="J7" s="41" t="s">
         <v>52</v>
       </c>
@@ -2978,7 +3006,7 @@
       <c r="G8" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="139"/>
+      <c r="I8" s="155"/>
       <c r="J8" s="7" t="s">
         <v>26</v>
       </c>
@@ -2986,7 +3014,7 @@
       <c r="L8" s="8"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="148" t="s">
+      <c r="B9" s="147" t="s">
         <v>133</v>
       </c>
       <c r="C9" s="36">
@@ -2995,7 +3023,7 @@
       <c r="D9" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="132" t="s">
+      <c r="E9" s="150" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="36">
@@ -3010,14 +3038,14 @@
       <c r="L9" s="9"/>
     </row>
     <row r="10" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="133"/>
+      <c r="B10" s="148"/>
       <c r="C10" s="32">
         <v>2</v>
       </c>
       <c r="D10" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="133"/>
+      <c r="E10" s="148"/>
       <c r="F10" s="32">
         <v>2</v>
       </c>
@@ -3029,14 +3057,14 @@
       </c>
     </row>
     <row r="11" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="134"/>
+      <c r="B11" s="149"/>
       <c r="C11" s="19">
         <v>1</v>
       </c>
       <c r="D11" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="134"/>
+      <c r="E11" s="149"/>
       <c r="F11" s="19">
         <v>3</v>
       </c>
@@ -3071,7 +3099,7 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="I13" s="138" t="s">
+      <c r="I13" s="154" t="s">
         <v>48</v>
       </c>
       <c r="J13" s="30" t="s">
@@ -3088,7 +3116,7 @@
       <c r="B14" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I14" s="138"/>
+      <c r="I14" s="154"/>
       <c r="J14" s="41" t="s">
         <v>55</v>
       </c>
@@ -3103,7 +3131,7 @@
       <c r="B15" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="I15" s="138"/>
+      <c r="I15" s="154"/>
       <c r="J15" s="41" t="s">
         <v>52</v>
       </c>
@@ -3127,7 +3155,7 @@
       <c r="G16" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="138"/>
+      <c r="I16" s="154"/>
       <c r="J16" s="41" t="s">
         <v>55</v>
       </c>
@@ -3139,7 +3167,7 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="143" t="s">
+      <c r="B17" s="159" t="s">
         <v>131</v>
       </c>
       <c r="C17" s="76">
@@ -3148,7 +3176,7 @@
       <c r="D17" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="135" t="s">
+      <c r="E17" s="151" t="s">
         <v>37</v>
       </c>
       <c r="F17" s="36">
@@ -3157,7 +3185,7 @@
       <c r="G17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I17" s="138"/>
+      <c r="I17" s="154"/>
       <c r="J17" s="39" t="s">
         <v>51</v>
       </c>
@@ -3169,14 +3197,14 @@
       </c>
     </row>
     <row r="18" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="144"/>
+      <c r="B18" s="160"/>
       <c r="C18" s="78">
         <v>2</v>
       </c>
       <c r="D18" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="136"/>
+      <c r="E18" s="152"/>
       <c r="F18" s="32">
         <v>2</v>
       </c>
@@ -3197,14 +3225,14 @@
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B19" s="144"/>
+      <c r="B19" s="160"/>
       <c r="C19" s="78">
         <v>3</v>
       </c>
       <c r="D19" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="146" t="s">
+      <c r="E19" s="162" t="s">
         <v>132</v>
       </c>
       <c r="F19" s="32">
@@ -3215,14 +3243,14 @@
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B20" s="144"/>
+      <c r="B20" s="160"/>
       <c r="C20" s="78">
         <v>4</v>
       </c>
       <c r="D20" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="136"/>
+      <c r="E20" s="152"/>
       <c r="F20" s="32">
         <v>2</v>
       </c>
@@ -3231,14 +3259,14 @@
       </c>
     </row>
     <row r="21" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="144"/>
+      <c r="B21" s="160"/>
       <c r="C21" s="78">
         <v>5</v>
       </c>
       <c r="D21" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="136"/>
+      <c r="E21" s="152"/>
       <c r="F21" s="32">
         <v>3</v>
       </c>
@@ -3250,14 +3278,14 @@
       </c>
     </row>
     <row r="22" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="144"/>
+      <c r="B22" s="160"/>
       <c r="C22" s="78">
         <v>6</v>
       </c>
       <c r="D22" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="136"/>
+      <c r="E22" s="152"/>
       <c r="F22" s="32">
         <v>4</v>
       </c>
@@ -3278,14 +3306,14 @@
       </c>
     </row>
     <row r="23" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="145"/>
+      <c r="B23" s="161"/>
       <c r="C23" s="80">
         <v>7</v>
       </c>
       <c r="D23" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="137"/>
+      <c r="E23" s="153"/>
       <c r="F23" s="19">
         <v>5</v>
       </c>
@@ -3304,7 +3332,7 @@
       </c>
     </row>
     <row r="24" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I24" s="138" t="s">
+      <c r="I24" s="154" t="s">
         <v>48</v>
       </c>
       <c r="J24" s="43" t="s">
@@ -3332,7 +3360,7 @@
       <c r="G25" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="I25" s="138"/>
+      <c r="I25" s="154"/>
       <c r="J25" s="44" t="s">
         <v>75</v>
       </c>
@@ -3342,7 +3370,7 @@
       </c>
     </row>
     <row r="26" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="147" t="s">
+      <c r="B26" s="163" t="s">
         <v>133</v>
       </c>
       <c r="C26" s="36">
@@ -3351,7 +3379,7 @@
       <c r="D26" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="135" t="s">
+      <c r="E26" s="151" t="s">
         <v>37</v>
       </c>
       <c r="F26" s="36">
@@ -3360,7 +3388,7 @@
       <c r="G26" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="I26" s="139"/>
+      <c r="I26" s="155"/>
       <c r="J26" s="7" t="s">
         <v>78</v>
       </c>
@@ -3370,14 +3398,14 @@
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B27" s="136"/>
+      <c r="B27" s="152"/>
       <c r="C27" s="32">
         <v>6</v>
       </c>
       <c r="D27" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="136"/>
+      <c r="E27" s="152"/>
       <c r="F27" s="32">
         <v>2</v>
       </c>
@@ -3386,14 +3414,14 @@
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B28" s="136"/>
+      <c r="B28" s="152"/>
       <c r="C28" s="32">
         <v>5</v>
       </c>
       <c r="D28" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="146" t="s">
+      <c r="E28" s="162" t="s">
         <v>132</v>
       </c>
       <c r="F28" s="32">
@@ -3404,14 +3432,14 @@
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B29" s="136"/>
+      <c r="B29" s="152"/>
       <c r="C29" s="32">
         <v>4</v>
       </c>
       <c r="D29" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="136"/>
+      <c r="E29" s="152"/>
       <c r="F29" s="32">
         <v>2</v>
       </c>
@@ -3420,14 +3448,14 @@
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B30" s="136"/>
+      <c r="B30" s="152"/>
       <c r="C30" s="32">
         <v>3</v>
       </c>
       <c r="D30" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="136"/>
+      <c r="E30" s="152"/>
       <c r="F30" s="32">
         <v>3</v>
       </c>
@@ -3436,14 +3464,14 @@
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B31" s="136"/>
+      <c r="B31" s="152"/>
       <c r="C31" s="32">
         <v>2</v>
       </c>
       <c r="D31" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="E31" s="136"/>
+      <c r="E31" s="152"/>
       <c r="F31" s="32">
         <v>4</v>
       </c>
@@ -3452,14 +3480,14 @@
       </c>
     </row>
     <row r="32" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="137"/>
+      <c r="B32" s="153"/>
       <c r="C32" s="19">
         <v>1</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E32" s="137"/>
+      <c r="E32" s="153"/>
       <c r="F32" s="19">
         <v>5</v>
       </c>
@@ -3494,7 +3522,7 @@
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="135" t="s">
+      <c r="B38" s="151" t="s">
         <v>36</v>
       </c>
       <c r="C38" s="36">
@@ -3508,7 +3536,7 @@
       <c r="G38" s="13"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B39" s="136"/>
+      <c r="B39" s="152"/>
       <c r="C39" s="32">
         <v>2</v>
       </c>
@@ -3520,14 +3548,14 @@
       <c r="G39" s="21"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B40" s="136"/>
+      <c r="B40" s="152"/>
       <c r="C40" s="32">
         <v>3</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E40" s="136" t="s">
+      <c r="E40" s="152" t="s">
         <v>69</v>
       </c>
       <c r="F40" s="32">
@@ -3538,14 +3566,14 @@
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B41" s="136"/>
+      <c r="B41" s="152"/>
       <c r="C41" s="32">
         <v>4</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E41" s="136"/>
+      <c r="E41" s="152"/>
       <c r="F41" s="32">
         <v>2</v>
       </c>
@@ -3554,7 +3582,7 @@
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="136"/>
+      <c r="B42" s="152"/>
       <c r="C42" s="32">
         <v>5</v>
       </c>
@@ -3566,7 +3594,7 @@
       <c r="G42" s="35"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B43" s="136"/>
+      <c r="B43" s="152"/>
       <c r="C43" s="32">
         <v>6</v>
       </c>
@@ -3578,7 +3606,7 @@
       <c r="G43" s="21"/>
     </row>
     <row r="44" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="137"/>
+      <c r="B44" s="153"/>
       <c r="C44" s="19">
         <v>7</v>
       </c>
@@ -3616,7 +3644,7 @@
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B50" s="135" t="s">
+      <c r="B50" s="151" t="s">
         <v>36</v>
       </c>
       <c r="C50" s="36">
@@ -3625,7 +3653,7 @@
       <c r="D50" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E50" s="135" t="s">
+      <c r="E50" s="151" t="s">
         <v>84</v>
       </c>
       <c r="F50" s="36" t="s">
@@ -3636,14 +3664,14 @@
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B51" s="136"/>
+      <c r="B51" s="152"/>
       <c r="C51" s="32">
         <v>2</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E51" s="136"/>
+      <c r="E51" s="152"/>
       <c r="F51" s="32">
         <v>7</v>
       </c>
@@ -3652,14 +3680,14 @@
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B52" s="136"/>
+      <c r="B52" s="152"/>
       <c r="C52" s="32">
         <v>3</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E52" s="136"/>
+      <c r="E52" s="152"/>
       <c r="F52" s="32">
         <v>9</v>
       </c>
@@ -3668,14 +3696,14 @@
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B53" s="136"/>
+      <c r="B53" s="152"/>
       <c r="C53" s="32">
         <v>4</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E53" s="136"/>
+      <c r="E53" s="152"/>
       <c r="F53" s="32">
         <v>3</v>
       </c>
@@ -3684,14 +3712,14 @@
       </c>
     </row>
     <row r="54" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="137"/>
+      <c r="B54" s="153"/>
       <c r="C54" s="19">
         <v>5</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E54" s="137"/>
+      <c r="E54" s="153"/>
       <c r="F54" s="19">
         <v>4</v>
       </c>
@@ -3701,6 +3729,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E28:E32"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="B50:B54"/>
@@ -3717,7 +3746,6 @@
     <mergeCell ref="E4:E6"/>
     <mergeCell ref="B26:B32"/>
     <mergeCell ref="E26:E27"/>
-    <mergeCell ref="E28:E32"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4075,7 +4103,7 @@
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C4" s="158" t="s">
+      <c r="C4" s="164" t="s">
         <v>100</v>
       </c>
       <c r="D4" s="47" t="s">
@@ -4093,22 +4121,22 @@
       <c r="H4" s="119" t="s">
         <v>96</v>
       </c>
-      <c r="L4" s="169"/>
-      <c r="M4" s="170"/>
-      <c r="N4" s="167" t="s">
+      <c r="L4" s="179"/>
+      <c r="M4" s="180"/>
+      <c r="N4" s="177" t="s">
         <v>153</v>
       </c>
-      <c r="O4" s="159" t="s">
+      <c r="O4" s="169" t="s">
         <v>140</v>
       </c>
-      <c r="P4" s="160"/>
-      <c r="Q4" s="151" t="s">
+      <c r="P4" s="170"/>
+      <c r="Q4" s="167" t="s">
         <v>143</v>
       </c>
-      <c r="R4" s="152"/>
+      <c r="R4" s="168"/>
     </row>
     <row r="5" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="156"/>
+      <c r="C5" s="165"/>
       <c r="D5" s="48" t="s">
         <v>97</v>
       </c>
@@ -4124,9 +4152,9 @@
       <c r="H5" s="120" t="s">
         <v>98</v>
       </c>
-      <c r="L5" s="171"/>
-      <c r="M5" s="172"/>
-      <c r="N5" s="168"/>
+      <c r="L5" s="181"/>
+      <c r="M5" s="182"/>
+      <c r="N5" s="178"/>
       <c r="O5" s="102" t="s">
         <v>145</v>
       </c>
@@ -4141,7 +4169,7 @@
       </c>
     </row>
     <row r="6" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="157"/>
+      <c r="C6" s="166"/>
       <c r="D6" s="49" t="s">
         <v>99</v>
       </c>
@@ -4160,10 +4188,10 @@
       <c r="H6" s="85" t="s">
         <v>91</v>
       </c>
-      <c r="L6" s="165" t="s">
+      <c r="L6" s="175" t="s">
         <v>134</v>
       </c>
-      <c r="M6" s="166"/>
+      <c r="M6" s="176"/>
       <c r="N6" s="50">
         <v>10</v>
       </c>
@@ -4183,7 +4211,7 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C7" s="158" t="s">
+      <c r="C7" s="164" t="s">
         <v>101</v>
       </c>
       <c r="D7" s="47" t="s">
@@ -4201,10 +4229,10 @@
       <c r="H7" s="119" t="s">
         <v>88</v>
       </c>
-      <c r="L7" s="163" t="s">
+      <c r="L7" s="173" t="s">
         <v>135</v>
       </c>
-      <c r="M7" s="164"/>
+      <c r="M7" s="174"/>
       <c r="N7" s="51">
         <v>7</v>
       </c>
@@ -4224,7 +4252,7 @@
       </c>
     </row>
     <row r="8" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="157"/>
+      <c r="C8" s="166"/>
       <c r="D8" s="49" t="s">
         <v>89</v>
       </c>
@@ -4243,10 +4271,10 @@
       <c r="H8" s="85" t="s">
         <v>90</v>
       </c>
-      <c r="L8" s="163" t="s">
+      <c r="L8" s="173" t="s">
         <v>136</v>
       </c>
-      <c r="M8" s="164"/>
+      <c r="M8" s="174"/>
       <c r="N8" s="51">
         <v>7</v>
       </c>
@@ -4266,7 +4294,7 @@
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C9" s="158" t="s">
+      <c r="C9" s="164" t="s">
         <v>102</v>
       </c>
       <c r="D9" s="47" t="s">
@@ -4282,10 +4310,10 @@
         <v>350</v>
       </c>
       <c r="H9" s="119"/>
-      <c r="L9" s="163" t="s">
+      <c r="L9" s="173" t="s">
         <v>137</v>
       </c>
-      <c r="M9" s="164"/>
+      <c r="M9" s="174"/>
       <c r="N9" s="51">
         <v>18</v>
       </c>
@@ -4305,7 +4333,7 @@
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C10" s="156"/>
+      <c r="C10" s="165"/>
       <c r="D10" s="48" t="s">
         <v>93</v>
       </c>
@@ -4324,10 +4352,10 @@
       <c r="H10" s="120" t="s">
         <v>88</v>
       </c>
-      <c r="L10" s="163" t="s">
+      <c r="L10" s="173" t="s">
         <v>138</v>
       </c>
-      <c r="M10" s="164"/>
+      <c r="M10" s="174"/>
       <c r="N10" s="51">
         <v>2500</v>
       </c>
@@ -4347,7 +4375,7 @@
       </c>
     </row>
     <row r="11" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="157"/>
+      <c r="C11" s="166"/>
       <c r="D11" s="49" t="s">
         <v>94</v>
       </c>
@@ -4366,10 +4394,10 @@
       <c r="H11" s="85" t="s">
         <v>91</v>
       </c>
-      <c r="L11" s="161" t="s">
+      <c r="L11" s="171" t="s">
         <v>139</v>
       </c>
-      <c r="M11" s="162"/>
+      <c r="M11" s="172"/>
       <c r="N11" s="52">
         <v>80</v>
       </c>
@@ -4430,10 +4458,10 @@
       </c>
       <c r="F14"/>
       <c r="G14"/>
-      <c r="L14" s="151" t="s">
+      <c r="L14" s="167" t="s">
         <v>140</v>
       </c>
-      <c r="M14" s="152"/>
+      <c r="M14" s="168"/>
       <c r="N14" s="109">
         <f>P12</f>
         <v>35</v>
@@ -4464,10 +4492,10 @@
       <c r="I15" s="119" t="s">
         <v>98</v>
       </c>
-      <c r="L15" s="153" t="s">
+      <c r="L15" s="185" t="s">
         <v>143</v>
       </c>
-      <c r="M15" s="154"/>
+      <c r="M15" s="186"/>
       <c r="N15" s="117">
         <f>R12</f>
         <v>2622</v>
@@ -4559,10 +4587,10 @@
       <c r="I18" s="85" t="s">
         <v>109</v>
       </c>
-      <c r="L18" s="151" t="s">
+      <c r="L18" s="167" t="s">
         <v>146</v>
       </c>
-      <c r="M18" s="152"/>
+      <c r="M18" s="168"/>
       <c r="N18" s="115">
         <v>1500</v>
       </c>
@@ -4581,10 +4609,10 @@
       <c r="F19"/>
       <c r="G19"/>
       <c r="I19" s="2"/>
-      <c r="L19" s="149" t="s">
+      <c r="L19" s="183" t="s">
         <v>140</v>
       </c>
-      <c r="M19" s="150"/>
+      <c r="M19" s="184"/>
       <c r="N19" s="110">
         <f>N$18/$N$14</f>
         <v>42.857142857142854</v>
@@ -4613,7 +4641,7 @@
       </c>
       <c r="H20" s="45"/>
       <c r="I20" s="2"/>
-      <c r="L20" s="155" t="s">
+      <c r="L20" s="187" t="s">
         <v>151</v>
       </c>
       <c r="M20" s="113">
@@ -4657,7 +4685,7 @@
       <c r="I21" s="119" t="s">
         <v>98</v>
       </c>
-      <c r="L21" s="156"/>
+      <c r="L21" s="165"/>
       <c r="M21" s="113">
         <v>40</v>
       </c>
@@ -4699,7 +4727,7 @@
       <c r="I22" s="120" t="s">
         <v>106</v>
       </c>
-      <c r="L22" s="156"/>
+      <c r="L22" s="165"/>
       <c r="M22" s="113">
         <v>60</v>
       </c>
@@ -4746,7 +4774,7 @@
       <c r="I23" s="120" t="s">
         <v>110</v>
       </c>
-      <c r="L23" s="156"/>
+      <c r="L23" s="165"/>
       <c r="M23" s="113">
         <v>80</v>
       </c>
@@ -4793,7 +4821,7 @@
       <c r="I24" s="85" t="s">
         <v>109</v>
       </c>
-      <c r="L24" s="157"/>
+      <c r="L24" s="166"/>
       <c r="M24" s="114">
         <v>100</v>
       </c>
@@ -4964,6 +4992,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="L20:L24"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C4:C6"/>
@@ -4977,11 +5010,6 @@
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="L4:M5"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="L20:L24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5014,10 +5042,10 @@
       <c r="D3" s="106" t="s">
         <v>158</v>
       </c>
-      <c r="E3" s="166" t="s">
+      <c r="E3" s="176" t="s">
         <v>159</v>
       </c>
-      <c r="F3" s="166"/>
+      <c r="F3" s="176"/>
       <c r="G3" s="50"/>
     </row>
     <row r="4" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -5111,10 +5139,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F28"/>
+  <dimension ref="B2:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5123,19 +5151,22 @@
     <col min="4" max="4" width="8.5" customWidth="1"/>
     <col min="5" max="5" width="10.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>120</v>
       </c>
@@ -5143,12 +5174,15 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="2:6" s="45" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" s="45" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="46" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H6" s="46" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C7" s="63" t="s">
         <v>126</v>
       </c>
@@ -5159,8 +5193,18 @@
         <v>122</v>
       </c>
       <c r="F7" s="65"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H7" s="89" t="s">
+        <v>200</v>
+      </c>
+      <c r="I7" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="J7" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="K7" s="65"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C8" s="66">
         <v>5</v>
       </c>
@@ -5171,8 +5215,18 @@
         <v>121</v>
       </c>
       <c r="F8" s="50"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H8" s="194">
+        <v>0.01</v>
+      </c>
+      <c r="I8" s="195" t="s">
+        <v>121</v>
+      </c>
+      <c r="J8" s="190">
+        <v>0.09</v>
+      </c>
+      <c r="K8" s="196"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C9" s="68">
         <v>4.9000000000000004</v>
       </c>
@@ -5183,8 +5237,18 @@
         <v>121</v>
       </c>
       <c r="F9" s="51"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H9" s="197">
+        <v>0.02</v>
+      </c>
+      <c r="I9" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="J9" s="71">
+        <v>0.09</v>
+      </c>
+      <c r="K9" s="73"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C10" s="68">
         <v>4.8</v>
       </c>
@@ -5195,8 +5259,18 @@
         <v>121</v>
       </c>
       <c r="F10" s="51"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H10" s="197">
+        <v>0.03</v>
+      </c>
+      <c r="I10" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="J10" s="71">
+        <v>0.09</v>
+      </c>
+      <c r="K10" s="73"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C11" s="68">
         <v>4.7</v>
       </c>
@@ -5207,8 +5281,18 @@
         <v>121</v>
       </c>
       <c r="F11" s="51"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H11" s="197">
+        <v>0.04</v>
+      </c>
+      <c r="I11" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="J11" s="71">
+        <v>0.09</v>
+      </c>
+      <c r="K11" s="73"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C12" s="68">
         <v>4.5999999999999996</v>
       </c>
@@ -5219,8 +5303,18 @@
         <v>121</v>
       </c>
       <c r="F12" s="51"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H12" s="197">
+        <v>0.05</v>
+      </c>
+      <c r="I12" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="J12" s="71">
+        <v>0.09</v>
+      </c>
+      <c r="K12" s="73"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C13" s="68">
         <v>4.5</v>
       </c>
@@ -5231,8 +5325,20 @@
         <v>121</v>
       </c>
       <c r="F13" s="51"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H13" s="198">
+        <v>0.06</v>
+      </c>
+      <c r="I13" s="199" t="s">
+        <v>121</v>
+      </c>
+      <c r="J13" s="200">
+        <v>0.09</v>
+      </c>
+      <c r="K13" s="201" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C14" s="68">
         <v>4.4000000000000004</v>
       </c>
@@ -5243,8 +5349,20 @@
         <v>121</v>
       </c>
       <c r="F14" s="51"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H14" s="198">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I14" s="199" t="s">
+        <v>121</v>
+      </c>
+      <c r="J14" s="200">
+        <v>0.09</v>
+      </c>
+      <c r="K14" s="201" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C15" s="68">
         <v>4.3</v>
       </c>
@@ -5255,8 +5373,20 @@
         <v>121</v>
       </c>
       <c r="F15" s="51"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H15" s="198">
+        <v>0.08</v>
+      </c>
+      <c r="I15" s="199" t="s">
+        <v>121</v>
+      </c>
+      <c r="J15" s="200">
+        <v>0.09</v>
+      </c>
+      <c r="K15" s="201" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C16" s="70">
         <v>4.2</v>
       </c>
@@ -5267,8 +5397,18 @@
         <v>121</v>
       </c>
       <c r="F16" s="73"/>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="H16" s="197">
+        <v>0.09</v>
+      </c>
+      <c r="I16" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="J16" s="71">
+        <v>0.09</v>
+      </c>
+      <c r="K16" s="73"/>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C17" s="70">
         <v>4.0999999999999996</v>
       </c>
@@ -5279,8 +5419,18 @@
         <v>121</v>
       </c>
       <c r="F17" s="73"/>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="H17" s="197">
+        <v>0.1</v>
+      </c>
+      <c r="I17" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="J17" s="71">
+        <v>0.09</v>
+      </c>
+      <c r="K17" s="73"/>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C18" s="70">
         <v>4</v>
       </c>
@@ -5291,8 +5441,18 @@
         <v>121</v>
       </c>
       <c r="F18" s="73"/>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="H18" s="197">
+        <v>0.11</v>
+      </c>
+      <c r="I18" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="J18" s="71">
+        <v>0.09</v>
+      </c>
+      <c r="K18" s="73"/>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C19" s="70">
         <v>3.9</v>
       </c>
@@ -5303,8 +5463,18 @@
         <v>121</v>
       </c>
       <c r="F19" s="73"/>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="H19" s="197">
+        <v>0.12</v>
+      </c>
+      <c r="I19" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="J19" s="71">
+        <v>0.09</v>
+      </c>
+      <c r="K19" s="73"/>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C20" s="70">
         <v>3.8</v>
       </c>
@@ -5315,8 +5485,18 @@
         <v>121</v>
       </c>
       <c r="F20" s="73"/>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="H20" s="197">
+        <v>0.13</v>
+      </c>
+      <c r="I20" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="J20" s="71">
+        <v>0.09</v>
+      </c>
+      <c r="K20" s="73"/>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C21" s="70">
         <v>3.7</v>
       </c>
@@ -5327,8 +5507,18 @@
         <v>121</v>
       </c>
       <c r="F21" s="73"/>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="H21" s="197">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I21" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="J21" s="71">
+        <v>0.09</v>
+      </c>
+      <c r="K21" s="73"/>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C22" s="70">
         <v>3.6</v>
       </c>
@@ -5339,8 +5529,18 @@
         <v>121</v>
       </c>
       <c r="F22" s="73"/>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="H22" s="197">
+        <v>0.15</v>
+      </c>
+      <c r="I22" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="J22" s="71">
+        <v>0.09</v>
+      </c>
+      <c r="K22" s="73"/>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C23" s="70">
         <v>3.5</v>
       </c>
@@ -5351,8 +5551,18 @@
         <v>121</v>
       </c>
       <c r="F23" s="73"/>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="H23" s="197">
+        <v>0.16</v>
+      </c>
+      <c r="I23" s="72" t="s">
+        <v>121</v>
+      </c>
+      <c r="J23" s="71">
+        <v>0.09</v>
+      </c>
+      <c r="K23" s="73"/>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C24" s="70">
         <v>3.4</v>
       </c>
@@ -5363,8 +5573,20 @@
         <v>121</v>
       </c>
       <c r="F24" s="73"/>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="H24" s="191">
+        <v>0.17</v>
+      </c>
+      <c r="I24" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="J24" s="192">
+        <v>0.09</v>
+      </c>
+      <c r="K24" s="51" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C25" s="68">
         <v>3.3</v>
       </c>
@@ -5375,8 +5597,18 @@
         <v>121</v>
       </c>
       <c r="F25" s="51"/>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="H25" s="191">
+        <v>0.18</v>
+      </c>
+      <c r="I25" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="J25" s="192">
+        <v>0.09</v>
+      </c>
+      <c r="K25" s="51"/>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C26" s="68">
         <v>3.2</v>
       </c>
@@ -5387,8 +5619,18 @@
         <v>121</v>
       </c>
       <c r="F26" s="51"/>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="H26" s="191">
+        <v>0.19</v>
+      </c>
+      <c r="I26" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="J26" s="192">
+        <v>0.09</v>
+      </c>
+      <c r="K26" s="51"/>
+    </row>
+    <row r="27" spans="3:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C27" s="68">
         <v>3.1</v>
       </c>
@@ -5401,8 +5643,18 @@
       <c r="F27" s="51" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="28" spans="3:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H27" s="139">
+        <v>0.2</v>
+      </c>
+      <c r="I27" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="J27" s="193">
+        <v>0.09</v>
+      </c>
+      <c r="K27" s="52"/>
+    </row>
+    <row r="28" spans="3:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C28" s="74">
         <v>3</v>
       </c>
@@ -5422,10 +5674,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:G28"/>
+  <dimension ref="B4:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5435,14 +5687,14 @@
     <col min="7" max="7" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="46" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="175"/>
-      <c r="C5" s="176"/>
+    <row r="5" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="132"/>
+      <c r="C5" s="133"/>
       <c r="D5" s="63" t="s">
         <v>191</v>
       </c>
@@ -5452,15 +5704,19 @@
       <c r="F5" s="90" t="s">
         <v>193</v>
       </c>
-      <c r="G5" s="177" t="s">
+      <c r="G5" s="134" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="158" t="s">
+      <c r="J5" t="s">
+        <v>195</v>
+      </c>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B6" s="164" t="s">
         <v>175</v>
       </c>
-      <c r="C6" s="186" t="s">
+      <c r="C6" s="143" t="s">
         <v>173</v>
       </c>
       <c r="D6" s="123">
@@ -5472,16 +5728,33 @@
       <c r="F6" s="50">
         <v>4</v>
       </c>
-      <c r="G6" s="178" t="s">
+      <c r="G6" s="135" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="156"/>
-      <c r="C7" s="184" t="s">
+      <c r="J6" s="45"/>
+      <c r="K6" s="141" t="s">
+        <v>180</v>
+      </c>
+      <c r="L6" s="141" t="s">
+        <v>196</v>
+      </c>
+      <c r="M6" s="141" t="s">
+        <v>197</v>
+      </c>
+      <c r="N6" s="45"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B7" s="165"/>
+      <c r="C7" s="141" t="s">
         <v>174</v>
       </c>
-      <c r="D7" s="187">
+      <c r="D7" s="144">
         <v>2.5</v>
       </c>
       <c r="E7" s="72">
@@ -5490,16 +5763,32 @@
       <c r="F7" s="73">
         <v>2.5</v>
       </c>
-      <c r="G7" s="188" t="s">
+      <c r="G7" s="145" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="156"/>
-      <c r="C8" s="184" t="s">
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>200</v>
+      </c>
+      <c r="L7">
+        <v>0.2</v>
+      </c>
+      <c r="M7" s="146">
+        <v>363.7</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="R7">
+        <v>2.41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="165"/>
+      <c r="C8" s="141" t="s">
         <v>177</v>
       </c>
-      <c r="D8" s="181">
+      <c r="D8" s="138">
         <f>D6*D7</f>
         <v>10</v>
       </c>
@@ -5511,18 +5800,35 @@
         <f>F6*F7</f>
         <v>10</v>
       </c>
-      <c r="G8" s="179" t="s">
+      <c r="G8" s="136" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="156" t="s">
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>200</v>
+      </c>
+      <c r="L8" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M8" s="146">
+        <v>360.9</v>
+      </c>
+      <c r="N8"/>
+      <c r="O8" s="2"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B9" s="165" t="s">
         <v>176</v>
       </c>
-      <c r="C9" s="184" t="s">
+      <c r="C9" s="141" t="s">
         <v>173</v>
       </c>
-      <c r="D9" s="181">
+      <c r="D9" s="138">
         <v>8</v>
       </c>
       <c r="E9" s="48">
@@ -5531,16 +5837,29 @@
       <c r="F9" s="51">
         <v>8</v>
       </c>
-      <c r="G9" s="179" t="s">
+      <c r="G9" s="136" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="156"/>
-      <c r="C10" s="184" t="s">
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>230</v>
+      </c>
+      <c r="L9" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M9" s="146">
+        <v>419</v>
+      </c>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B10" s="165"/>
+      <c r="C10" s="141" t="s">
         <v>174</v>
       </c>
-      <c r="D10" s="181">
+      <c r="D10" s="138">
         <f>D8/D9</f>
         <v>1.25</v>
       </c>
@@ -5552,18 +5871,31 @@
         <f>F8/F9</f>
         <v>1.25</v>
       </c>
-      <c r="G10" s="179" t="s">
+      <c r="G10" s="136" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="156" t="s">
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>230</v>
+      </c>
+      <c r="L10" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M10" s="146">
+        <v>413.2</v>
+      </c>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B11" s="165" t="s">
         <v>178</v>
       </c>
-      <c r="C11" s="184" t="s">
+      <c r="C11" s="141" t="s">
         <v>179</v>
       </c>
-      <c r="D11" s="181">
+      <c r="D11" s="138">
         <v>5</v>
       </c>
       <c r="E11" s="48">
@@ -5572,16 +5904,29 @@
       <c r="F11" s="51">
         <v>5</v>
       </c>
-      <c r="G11" s="179" t="s">
+      <c r="G11" s="136" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="156"/>
-      <c r="C12" s="184" t="s">
+      <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>230</v>
+      </c>
+      <c r="L11" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M11" s="146">
+        <v>419</v>
+      </c>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="165"/>
+      <c r="C12" s="141" t="s">
         <v>180</v>
       </c>
-      <c r="D12" s="181">
+      <c r="D12" s="138">
         <v>200</v>
       </c>
       <c r="E12" s="48">
@@ -5590,14 +5935,32 @@
       <c r="F12" s="51">
         <v>250</v>
       </c>
-      <c r="G12" s="179"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="156"/>
-      <c r="C13" s="184" t="s">
+      <c r="G12" s="136"/>
+      <c r="J12">
+        <v>7</v>
+      </c>
+      <c r="K12">
+        <v>250</v>
+      </c>
+      <c r="L12" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M12" s="146">
+        <v>461</v>
+      </c>
+      <c r="N12">
+        <v>443</v>
+      </c>
+      <c r="O12" s="129" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B13" s="165"/>
+      <c r="C13" s="141" t="s">
         <v>181</v>
       </c>
-      <c r="D13" s="181">
+      <c r="D13" s="138">
         <f>D12*7</f>
         <v>1400</v>
       </c>
@@ -5609,16 +5972,29 @@
         <f>F12*7</f>
         <v>1750</v>
       </c>
-      <c r="G13" s="179" t="s">
+      <c r="G13" s="136" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="156"/>
-      <c r="C14" s="184" t="s">
+      <c r="J13">
+        <v>8</v>
+      </c>
+      <c r="K13">
+        <v>250</v>
+      </c>
+      <c r="L13" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M13" s="146">
+        <v>458</v>
+      </c>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="2:18" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="165"/>
+      <c r="C14" s="141" t="s">
         <v>183</v>
       </c>
-      <c r="D14" s="181">
+      <c r="D14" s="138">
         <f>D13/D11</f>
         <v>280</v>
       </c>
@@ -5630,18 +6006,35 @@
         <f>F13/F11</f>
         <v>350</v>
       </c>
-      <c r="G14" s="179" t="s">
+      <c r="G14" s="136" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="156" t="s">
+      <c r="J14">
+        <v>9</v>
+      </c>
+      <c r="K14">
+        <v>250</v>
+      </c>
+      <c r="L14" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="M14" s="146">
+        <v>460</v>
+      </c>
+      <c r="N14"/>
+      <c r="O14" s="2"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B15" s="165" t="s">
         <v>182</v>
       </c>
-      <c r="C15" s="184" t="s">
+      <c r="C15" s="141" t="s">
         <v>173</v>
       </c>
-      <c r="D15" s="181">
+      <c r="D15" s="138">
         <f>D9*D14</f>
         <v>2240</v>
       </c>
@@ -5653,16 +6046,16 @@
         <f>F9*F14</f>
         <v>2800</v>
       </c>
-      <c r="G15" s="179" t="s">
+      <c r="G15" s="136" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="157"/>
-      <c r="C16" s="185" t="s">
+    <row r="16" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="166"/>
+      <c r="C16" s="142" t="s">
         <v>174</v>
       </c>
-      <c r="D16" s="182">
+      <c r="D16" s="139">
         <f>D8/D15*1000</f>
         <v>4.4642857142857144</v>
       </c>
@@ -5670,155 +6063,53 @@
         <f>E8/E15*1000</f>
         <v>3.8819875776397517</v>
       </c>
-      <c r="F16" s="183">
+      <c r="F16" s="140">
         <f>F8/F15*1000</f>
         <v>3.5714285714285712</v>
       </c>
-      <c r="G16" s="180" t="s">
+      <c r="G16" s="137" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="184" t="s">
-        <v>180</v>
-      </c>
-      <c r="D20" s="184" t="s">
-        <v>196</v>
-      </c>
-      <c r="E20" s="184" t="s">
-        <v>197</v>
-      </c>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>200</v>
-      </c>
-      <c r="D21">
-        <v>0.2</v>
-      </c>
-      <c r="E21" s="189">
-        <v>363.7</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22">
-        <v>200</v>
-      </c>
-      <c r="D22" s="45">
-        <v>0.2</v>
-      </c>
-      <c r="E22" s="189">
-        <v>360.9</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23">
-        <v>3</v>
-      </c>
-      <c r="C23">
-        <v>230</v>
-      </c>
-      <c r="D23" s="45">
-        <v>0.2</v>
-      </c>
-      <c r="E23" s="189">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24">
-        <v>5</v>
-      </c>
-      <c r="C24">
-        <v>230</v>
-      </c>
-      <c r="D24" s="45">
-        <v>0.2</v>
-      </c>
-      <c r="E24" s="189">
-        <v>413.2</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25">
-        <v>6</v>
-      </c>
-      <c r="C25">
-        <v>230</v>
-      </c>
-      <c r="D25" s="45">
-        <v>0.2</v>
-      </c>
-      <c r="E25" s="189">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26">
-        <v>7</v>
-      </c>
-      <c r="C26">
-        <v>250</v>
-      </c>
-      <c r="D26" s="45">
-        <v>0.2</v>
-      </c>
-      <c r="E26" s="189">
-        <v>461</v>
-      </c>
-      <c r="F26">
-        <v>443</v>
-      </c>
-      <c r="G26" s="129" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27">
-        <v>8</v>
-      </c>
-      <c r="C27">
-        <v>250</v>
-      </c>
-      <c r="D27" s="45">
-        <v>0.2</v>
-      </c>
-      <c r="E27" s="189">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28">
-        <v>9</v>
-      </c>
-      <c r="C28">
-        <v>250</v>
-      </c>
-      <c r="D28" s="45">
-        <v>0.2</v>
-      </c>
-      <c r="E28" s="189">
-        <v>460</v>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="165" t="s">
+        <v>199</v>
+      </c>
+      <c r="C17" s="141" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="166"/>
+      <c r="C18" s="142" t="s">
+        <v>174</v>
+      </c>
+      <c r="D18">
+        <v>2.41</v>
+      </c>
+      <c r="E18">
+        <v>2.41</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" s="45" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>2.33</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B17:B18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5848,17 +6139,17 @@
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C3" s="174" t="s">
+      <c r="C3" s="189" t="s">
         <v>166</v>
       </c>
-      <c r="D3" s="174"/>
+      <c r="D3" s="189"/>
       <c r="E3" t="s">
         <v>169</v>
       </c>
-      <c r="F3" s="173" t="s">
+      <c r="F3" s="188" t="s">
         <v>163</v>
       </c>
-      <c r="G3" s="173"/>
+      <c r="G3" s="188"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">

</xml_diff>